<commit_message>
Output Teacher Overview + Appearance
Alyssa created the output teacher overview and I made some changes to it so that it is readable.
</commit_message>
<xml_diff>
--- a/FYDP_ModV1/flamborough_feb6.xlsx
+++ b/FYDP_ModV1/flamborough_feb6.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\fydp\FYDP_ModV1\"/>
     </mc:Choice>
@@ -18,6 +18,7 @@
     <sheet name="INPUT SHEET 3" sheetId="4" r:id="rId3"/>
     <sheet name="OUTPUT SHEET" sheetId="3" r:id="rId4"/>
     <sheet name="dropdown lists (HIDE)" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="MasterSchedule2020.02.10.18.29." r:id="rId11" sheetId="6"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId6"/>
@@ -27,7 +28,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="179">
   <si>
     <t>Schedule Title</t>
   </si>
@@ -352,12 +353,247 @@
   <si>
     <t>Jk/Sk</t>
   </si>
+  <si>
+    <t>Jk/Sk / Language</t>
+  </si>
+  <si>
+    <t>Jk/Sk / Phys-Ed</t>
+  </si>
+  <si>
+    <t>Jk/Sk / Social-Studies</t>
+  </si>
+  <si>
+    <t>Jk/Sk / Science</t>
+  </si>
+  <si>
+    <t>Jk/Sk / Math</t>
+  </si>
+  <si>
+    <t>class1/2 / Math</t>
+  </si>
+  <si>
+    <t>class1/2 / Science</t>
+  </si>
+  <si>
+    <t>class1/2 / Phys-Ed</t>
+  </si>
+  <si>
+    <t>class1/2 / Language</t>
+  </si>
+  <si>
+    <t>class1/2 / Art</t>
+  </si>
+  <si>
+    <t>class3A / Math</t>
+  </si>
+  <si>
+    <t>class3A / Science</t>
+  </si>
+  <si>
+    <t>class3A / Language</t>
+  </si>
+  <si>
+    <t>class3A / Social-Studies</t>
+  </si>
+  <si>
+    <t>class3A / Art</t>
+  </si>
+  <si>
+    <t>class3A / Phys-Ed</t>
+  </si>
+  <si>
+    <t>class4/5 / Math</t>
+  </si>
+  <si>
+    <t>class4/5 / Language</t>
+  </si>
+  <si>
+    <t>class4/5 / Art</t>
+  </si>
+  <si>
+    <t>class4/5 / Social-Studies</t>
+  </si>
+  <si>
+    <t>class4/5 / Phys-Ed</t>
+  </si>
+  <si>
+    <t>class4/5 / Science</t>
+  </si>
+  <si>
+    <t>class6/7 / Music</t>
+  </si>
+  <si>
+    <t>class6b / Science</t>
+  </si>
+  <si>
+    <t>class6b / Drama</t>
+  </si>
+  <si>
+    <t>class6b / Language</t>
+  </si>
+  <si>
+    <t>class6b / Math</t>
+  </si>
+  <si>
+    <t>class6b / Phys-Ed</t>
+  </si>
+  <si>
+    <t>class6b / Social-Studies</t>
+  </si>
+  <si>
+    <t>class6b / Art</t>
+  </si>
+  <si>
+    <t>class6/7 / Math</t>
+  </si>
+  <si>
+    <t>class6/7 / Language</t>
+  </si>
+  <si>
+    <t>class6/7 / Science</t>
+  </si>
+  <si>
+    <t>class6/7 / Drama</t>
+  </si>
+  <si>
+    <t>class6/7 / Art</t>
+  </si>
+  <si>
+    <t>class6/7 / Phys-Ed</t>
+  </si>
+  <si>
+    <t>class6/7 / Social-Studies</t>
+  </si>
+  <si>
+    <t>class7a / Science</t>
+  </si>
+  <si>
+    <t>class7a / Language</t>
+  </si>
+  <si>
+    <t>class7a / Math</t>
+  </si>
+  <si>
+    <t>class7a / Phys-Ed</t>
+  </si>
+  <si>
+    <t>Jk/Sk / Art</t>
+  </si>
+  <si>
+    <t>class7a / Art</t>
+  </si>
+  <si>
+    <t>class7a / Social-Studies</t>
+  </si>
+  <si>
+    <t>class8a / Math</t>
+  </si>
+  <si>
+    <t>class8a / Language</t>
+  </si>
+  <si>
+    <t>class8a / Social-Studies</t>
+  </si>
+  <si>
+    <t>class8a / Science</t>
+  </si>
+  <si>
+    <t>class8a / Drama</t>
+  </si>
+  <si>
+    <t>class8a / Music</t>
+  </si>
+  <si>
+    <t>class8a / Phys-Ed</t>
+  </si>
+  <si>
+    <t>Jk/Sk / Music</t>
+  </si>
+  <si>
+    <t>class1/2 / Music</t>
+  </si>
+  <si>
+    <t>class6a / Drama</t>
+  </si>
+  <si>
+    <t>class1/2 / Drama</t>
+  </si>
+  <si>
+    <t>class6a / Science</t>
+  </si>
+  <si>
+    <t>class3A / Music</t>
+  </si>
+  <si>
+    <t>class7a / Music</t>
+  </si>
+  <si>
+    <t>class6a / Music</t>
+  </si>
+  <si>
+    <t>class1/2 / Social-Studies</t>
+  </si>
+  <si>
+    <t>class3A / Drama</t>
+  </si>
+  <si>
+    <t>class6b / Music</t>
+  </si>
+  <si>
+    <t>Jk/Sk / Drama</t>
+  </si>
+  <si>
+    <t>class4/5 / Music</t>
+  </si>
+  <si>
+    <t>class6a / Social-Studies</t>
+  </si>
+  <si>
+    <t>class6a / Art</t>
+  </si>
+  <si>
+    <t>class8a / Art</t>
+  </si>
+  <si>
+    <t>class6a / Language</t>
+  </si>
+  <si>
+    <t>class6b / French</t>
+  </si>
+  <si>
+    <t>class6a / Math</t>
+  </si>
+  <si>
+    <t>class4/5 / French</t>
+  </si>
+  <si>
+    <t>class6a / Phys-Ed</t>
+  </si>
+  <si>
+    <t>class4/5 / Drama</t>
+  </si>
+  <si>
+    <t>class6/7 / French</t>
+  </si>
+  <si>
+    <t>class6a / French</t>
+  </si>
+  <si>
+    <t>class8a / French</t>
+  </si>
+  <si>
+    <t>class7a / French</t>
+  </si>
+  <si>
+    <t>class7a / Drama</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -388,8 +624,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,12 +651,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-0.249977111117893" rgb="E7E6E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="64"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -476,11 +737,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -718,6 +1027,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2202,13 +2518,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="10.625" style="11"/>
-    <col min="3" max="3" width="13.125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="12.125" style="11" customWidth="1"/>
-    <col min="5" max="9" width="10.625" style="11"/>
-    <col min="10" max="10" width="0" style="11" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.625" style="11"/>
+    <col min="1" max="1" customWidth="true" style="11" width="28.875" collapsed="false"/>
+    <col min="2" max="2" style="11" width="10.625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="11" width="13.125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="11" width="12.125" collapsed="false"/>
+    <col min="5" max="9" style="11" width="10.625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" hidden="true" style="11" width="0.0" collapsed="false"/>
+    <col min="11" max="16384" style="11" width="10.625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -3628,9 +3944,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="11" customWidth="1"/>
-    <col min="2" max="2" width="12" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="10.625" style="11"/>
+    <col min="1" max="1" customWidth="true" style="11" width="22.5" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="11" width="12.0" collapsed="false"/>
+    <col min="3" max="16384" style="11" width="10.625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -9054,9 +9370,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.125" style="11" customWidth="1"/>
-    <col min="2" max="11" width="14.125" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="10.625" style="11"/>
+    <col min="1" max="1" customWidth="true" style="11" width="19.125" collapsed="false"/>
+    <col min="2" max="11" customWidth="true" style="11" width="14.125" collapsed="false"/>
+    <col min="12" max="16384" style="11" width="10.625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
@@ -14413,8 +14729,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="21.875" customWidth="1"/>
-    <col min="9" max="38" width="16.875" style="6" customWidth="1"/>
+    <col min="2" max="6" customWidth="true" width="21.875" collapsed="false"/>
+    <col min="9" max="38" customWidth="true" style="6" width="16.875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -14628,7 +14944,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.5" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -15091,4 +15407,1656 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="B1:AF18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="C1" t="s" s="77">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s" s="77">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s" s="77">
+        <v>5</v>
+      </c>
+      <c r="U1" t="s" s="77">
+        <v>6</v>
+      </c>
+      <c r="AA1" t="s" s="77">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s" s="76">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s" s="76">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s" s="76">
+        <v>102</v>
+      </c>
+      <c r="F3" t="s" s="76">
+        <v>103</v>
+      </c>
+      <c r="G3" t="s" s="76">
+        <v>104</v>
+      </c>
+      <c r="H3" t="s" s="76">
+        <v>105</v>
+      </c>
+      <c r="I3" t="s" s="76">
+        <v>105</v>
+      </c>
+      <c r="J3" t="s" s="76">
+        <v>104</v>
+      </c>
+      <c r="K3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" t="s" s="76">
+        <v>103</v>
+      </c>
+      <c r="M3" t="s" s="76">
+        <v>101</v>
+      </c>
+      <c r="N3" t="s" s="76">
+        <v>101</v>
+      </c>
+      <c r="O3" t="s" s="76">
+        <v>105</v>
+      </c>
+      <c r="P3" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q3" t="s" s="76">
+        <v>104</v>
+      </c>
+      <c r="R3" t="s" s="76">
+        <v>103</v>
+      </c>
+      <c r="S3" t="s" s="76">
+        <v>101</v>
+      </c>
+      <c r="T3" t="s" s="76">
+        <v>101</v>
+      </c>
+      <c r="U3" t="s" s="76">
+        <v>105</v>
+      </c>
+      <c r="V3" t="s" s="76">
+        <v>102</v>
+      </c>
+      <c r="W3" t="s" s="76">
+        <v>101</v>
+      </c>
+      <c r="X3" t="s" s="76">
+        <v>101</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA3" t="s" s="76">
+        <v>101</v>
+      </c>
+      <c r="AB3" t="s" s="76">
+        <v>101</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD3" t="s" s="76">
+        <v>103</v>
+      </c>
+      <c r="AE3" t="s" s="76">
+        <v>104</v>
+      </c>
+      <c r="AF3" t="s" s="76">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s" s="76">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s" s="76">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s" s="76">
+        <v>108</v>
+      </c>
+      <c r="F4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" t="s" s="76">
+        <v>109</v>
+      </c>
+      <c r="H4" t="s" s="76">
+        <v>109</v>
+      </c>
+      <c r="I4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" t="s" s="76">
+        <v>108</v>
+      </c>
+      <c r="K4" t="s" s="76">
+        <v>109</v>
+      </c>
+      <c r="L4" t="s" s="76">
+        <v>109</v>
+      </c>
+      <c r="M4" t="s" s="76">
+        <v>107</v>
+      </c>
+      <c r="N4" t="s" s="76">
+        <v>106</v>
+      </c>
+      <c r="O4" t="s" s="76">
+        <v>109</v>
+      </c>
+      <c r="P4" t="s" s="76">
+        <v>109</v>
+      </c>
+      <c r="Q4" t="s" s="76">
+        <v>108</v>
+      </c>
+      <c r="R4" t="s" s="76">
+        <v>107</v>
+      </c>
+      <c r="S4" t="s">
+        <v>99</v>
+      </c>
+      <c r="T4" t="s" s="76">
+        <v>106</v>
+      </c>
+      <c r="U4" t="s" s="76">
+        <v>106</v>
+      </c>
+      <c r="V4" t="s" s="76">
+        <v>108</v>
+      </c>
+      <c r="W4" t="s" s="76">
+        <v>107</v>
+      </c>
+      <c r="X4" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y4" t="s" s="76">
+        <v>109</v>
+      </c>
+      <c r="Z4" t="s" s="76">
+        <v>109</v>
+      </c>
+      <c r="AA4" t="s" s="76">
+        <v>109</v>
+      </c>
+      <c r="AB4" t="s" s="76">
+        <v>109</v>
+      </c>
+      <c r="AC4" t="s" s="76">
+        <v>110</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE4" t="s" s="76">
+        <v>107</v>
+      </c>
+      <c r="AF4" t="s" s="76">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s" s="76">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s" s="76">
+        <v>112</v>
+      </c>
+      <c r="E5" t="s" s="76">
+        <v>113</v>
+      </c>
+      <c r="F5" t="s" s="76">
+        <v>113</v>
+      </c>
+      <c r="G5" t="s" s="76">
+        <v>114</v>
+      </c>
+      <c r="H5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" t="s" s="76">
+        <v>111</v>
+      </c>
+      <c r="J5" t="s" s="76">
+        <v>115</v>
+      </c>
+      <c r="K5" t="s" s="76">
+        <v>113</v>
+      </c>
+      <c r="L5" t="s" s="76">
+        <v>113</v>
+      </c>
+      <c r="M5" t="s" s="76">
+        <v>116</v>
+      </c>
+      <c r="N5" t="s">
+        <v>99</v>
+      </c>
+      <c r="O5" t="s" s="76">
+        <v>111</v>
+      </c>
+      <c r="P5" t="s" s="76">
+        <v>114</v>
+      </c>
+      <c r="Q5" t="s" s="76">
+        <v>113</v>
+      </c>
+      <c r="R5" t="s" s="76">
+        <v>113</v>
+      </c>
+      <c r="S5" t="s" s="76">
+        <v>115</v>
+      </c>
+      <c r="T5" t="s">
+        <v>99</v>
+      </c>
+      <c r="U5" t="s" s="76">
+        <v>111</v>
+      </c>
+      <c r="V5" t="s" s="76">
+        <v>115</v>
+      </c>
+      <c r="W5" t="s" s="76">
+        <v>113</v>
+      </c>
+      <c r="X5" t="s" s="76">
+        <v>113</v>
+      </c>
+      <c r="Y5" t="s" s="76">
+        <v>115</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA5" t="s" s="76">
+        <v>111</v>
+      </c>
+      <c r="AB5" t="s" s="76">
+        <v>112</v>
+      </c>
+      <c r="AC5" t="s" s="76">
+        <v>113</v>
+      </c>
+      <c r="AD5" t="s" s="76">
+        <v>113</v>
+      </c>
+      <c r="AE5" t="s" s="76">
+        <v>114</v>
+      </c>
+      <c r="AF5" t="s" s="76">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s" s="76">
+        <v>117</v>
+      </c>
+      <c r="D6" t="s" s="76">
+        <v>118</v>
+      </c>
+      <c r="E6" t="s" s="76">
+        <v>119</v>
+      </c>
+      <c r="F6" t="s" s="76">
+        <v>120</v>
+      </c>
+      <c r="G6" t="s" s="76">
+        <v>118</v>
+      </c>
+      <c r="H6" t="s" s="76">
+        <v>121</v>
+      </c>
+      <c r="I6" t="s" s="76">
+        <v>117</v>
+      </c>
+      <c r="J6" t="s" s="76">
+        <v>118</v>
+      </c>
+      <c r="K6" t="s" s="76">
+        <v>122</v>
+      </c>
+      <c r="L6" t="s" s="76">
+        <v>121</v>
+      </c>
+      <c r="M6" t="s" s="76">
+        <v>118</v>
+      </c>
+      <c r="N6" t="s">
+        <v>99</v>
+      </c>
+      <c r="O6" t="s" s="76">
+        <v>122</v>
+      </c>
+      <c r="P6" t="s" s="76">
+        <v>118</v>
+      </c>
+      <c r="Q6" t="s" s="76">
+        <v>120</v>
+      </c>
+      <c r="R6" t="s">
+        <v>99</v>
+      </c>
+      <c r="S6" t="s">
+        <v>99</v>
+      </c>
+      <c r="T6" t="s" s="76">
+        <v>117</v>
+      </c>
+      <c r="U6" t="s" s="76">
+        <v>118</v>
+      </c>
+      <c r="V6" t="s" s="76">
+        <v>122</v>
+      </c>
+      <c r="W6" t="s">
+        <v>99</v>
+      </c>
+      <c r="X6" t="s" s="76">
+        <v>118</v>
+      </c>
+      <c r="Y6" t="s" s="76">
+        <v>123</v>
+      </c>
+      <c r="Z6" t="s" s="76">
+        <v>117</v>
+      </c>
+      <c r="AA6" t="s" s="76">
+        <v>117</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC6" t="s" s="76">
+        <v>122</v>
+      </c>
+      <c r="AD6" t="s" s="76">
+        <v>119</v>
+      </c>
+      <c r="AE6" t="s" s="76">
+        <v>118</v>
+      </c>
+      <c r="AF6" t="s" s="76">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s" s="76">
+        <v>124</v>
+      </c>
+      <c r="D7" t="s" s="76">
+        <v>125</v>
+      </c>
+      <c r="E7" t="s" s="76">
+        <v>126</v>
+      </c>
+      <c r="F7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" t="s" s="76">
+        <v>125</v>
+      </c>
+      <c r="H7" t="s" s="76">
+        <v>127</v>
+      </c>
+      <c r="I7" t="s" s="76">
+        <v>128</v>
+      </c>
+      <c r="J7" t="s" s="76">
+        <v>129</v>
+      </c>
+      <c r="K7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L7" t="s" s="76">
+        <v>130</v>
+      </c>
+      <c r="M7" t="s" s="76">
+        <v>126</v>
+      </c>
+      <c r="N7" t="s" s="76">
+        <v>127</v>
+      </c>
+      <c r="O7" t="s">
+        <v>99</v>
+      </c>
+      <c r="P7" t="s" s="76">
+        <v>126</v>
+      </c>
+      <c r="Q7" t="s" s="76">
+        <v>126</v>
+      </c>
+      <c r="R7" t="s" s="76">
+        <v>124</v>
+      </c>
+      <c r="S7" t="s" s="76">
+        <v>129</v>
+      </c>
+      <c r="T7" t="s" s="76">
+        <v>127</v>
+      </c>
+      <c r="U7" t="s" s="76">
+        <v>128</v>
+      </c>
+      <c r="V7" t="s" s="76">
+        <v>126</v>
+      </c>
+      <c r="W7" t="s" s="76">
+        <v>130</v>
+      </c>
+      <c r="X7" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y7" t="s" s="76">
+        <v>124</v>
+      </c>
+      <c r="Z7" t="s" s="76">
+        <v>127</v>
+      </c>
+      <c r="AA7" t="s" s="76">
+        <v>127</v>
+      </c>
+      <c r="AB7" t="s" s="76">
+        <v>124</v>
+      </c>
+      <c r="AC7" t="s" s="76">
+        <v>128</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE7" t="s" s="76">
+        <v>126</v>
+      </c>
+      <c r="AF7" t="s" s="76">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s" s="76">
+        <v>131</v>
+      </c>
+      <c r="D8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" t="s" s="76">
+        <v>132</v>
+      </c>
+      <c r="F8" t="s" s="76">
+        <v>132</v>
+      </c>
+      <c r="G8" t="s" s="76">
+        <v>133</v>
+      </c>
+      <c r="H8" t="s" s="76">
+        <v>134</v>
+      </c>
+      <c r="I8" t="s" s="76">
+        <v>132</v>
+      </c>
+      <c r="J8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K8" t="s" s="76">
+        <v>135</v>
+      </c>
+      <c r="L8" t="s" s="76">
+        <v>133</v>
+      </c>
+      <c r="M8" t="s" s="76">
+        <v>136</v>
+      </c>
+      <c r="N8" t="s" s="76">
+        <v>131</v>
+      </c>
+      <c r="O8" t="s">
+        <v>99</v>
+      </c>
+      <c r="P8" t="s" s="76">
+        <v>132</v>
+      </c>
+      <c r="Q8" t="s" s="76">
+        <v>135</v>
+      </c>
+      <c r="R8" t="s" s="76">
+        <v>137</v>
+      </c>
+      <c r="S8" t="s" s="76">
+        <v>133</v>
+      </c>
+      <c r="T8" t="s" s="76">
+        <v>131</v>
+      </c>
+      <c r="U8" t="s" s="76">
+        <v>132</v>
+      </c>
+      <c r="V8" t="s" s="76">
+        <v>132</v>
+      </c>
+      <c r="W8" t="s" s="76">
+        <v>133</v>
+      </c>
+      <c r="X8" t="s" s="76">
+        <v>137</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z8" t="s" s="76">
+        <v>131</v>
+      </c>
+      <c r="AA8" t="s" s="76">
+        <v>131</v>
+      </c>
+      <c r="AB8" t="s" s="76">
+        <v>135</v>
+      </c>
+      <c r="AC8" t="s" s="76">
+        <v>132</v>
+      </c>
+      <c r="AD8" t="s" s="76">
+        <v>134</v>
+      </c>
+      <c r="AE8" t="s" s="76">
+        <v>136</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s" s="76">
+        <v>138</v>
+      </c>
+      <c r="E9" t="s" s="76">
+        <v>139</v>
+      </c>
+      <c r="F9" t="s" s="76">
+        <v>139</v>
+      </c>
+      <c r="G9" t="s" s="76">
+        <v>139</v>
+      </c>
+      <c r="H9" t="s" s="76">
+        <v>140</v>
+      </c>
+      <c r="I9" t="s" s="76">
+        <v>140</v>
+      </c>
+      <c r="J9" t="s" s="76">
+        <v>141</v>
+      </c>
+      <c r="K9" t="s" s="76">
+        <v>142</v>
+      </c>
+      <c r="L9" t="s" s="76">
+        <v>139</v>
+      </c>
+      <c r="M9" t="s">
+        <v>99</v>
+      </c>
+      <c r="N9" t="s" s="76">
+        <v>139</v>
+      </c>
+      <c r="O9" t="s" s="76">
+        <v>138</v>
+      </c>
+      <c r="P9" t="s" s="76">
+        <v>141</v>
+      </c>
+      <c r="Q9" t="s" s="76">
+        <v>143</v>
+      </c>
+      <c r="R9" t="s">
+        <v>99</v>
+      </c>
+      <c r="S9" t="s" s="76">
+        <v>139</v>
+      </c>
+      <c r="T9" t="s" s="76">
+        <v>140</v>
+      </c>
+      <c r="U9" t="s" s="76">
+        <v>138</v>
+      </c>
+      <c r="V9" t="s" s="76">
+        <v>144</v>
+      </c>
+      <c r="W9" t="s" s="76">
+        <v>139</v>
+      </c>
+      <c r="X9" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y9" t="s" s="76">
+        <v>139</v>
+      </c>
+      <c r="Z9" t="s" s="76">
+        <v>140</v>
+      </c>
+      <c r="AA9" t="s" s="76">
+        <v>139</v>
+      </c>
+      <c r="AB9" t="s" s="76">
+        <v>143</v>
+      </c>
+      <c r="AC9" t="s" s="76">
+        <v>142</v>
+      </c>
+      <c r="AD9" t="s" s="76">
+        <v>144</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF9" t="s" s="76">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s" s="76">
+        <v>145</v>
+      </c>
+      <c r="D10" t="s" s="76">
+        <v>146</v>
+      </c>
+      <c r="E10" t="s" s="76">
+        <v>146</v>
+      </c>
+      <c r="F10" t="s" s="76">
+        <v>147</v>
+      </c>
+      <c r="G10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" t="s" s="76">
+        <v>148</v>
+      </c>
+      <c r="I10" t="s" s="76">
+        <v>148</v>
+      </c>
+      <c r="J10" t="s" s="76">
+        <v>146</v>
+      </c>
+      <c r="K10" t="s" s="76">
+        <v>149</v>
+      </c>
+      <c r="L10" t="s" s="76">
+        <v>150</v>
+      </c>
+      <c r="M10" t="s">
+        <v>99</v>
+      </c>
+      <c r="N10" t="s" s="76">
+        <v>145</v>
+      </c>
+      <c r="O10" t="s" s="76">
+        <v>145</v>
+      </c>
+      <c r="P10" t="s" s="76">
+        <v>147</v>
+      </c>
+      <c r="Q10" t="s" s="76">
+        <v>146</v>
+      </c>
+      <c r="R10" t="s" s="76">
+        <v>146</v>
+      </c>
+      <c r="S10" t="s" s="76">
+        <v>146</v>
+      </c>
+      <c r="T10" t="s">
+        <v>99</v>
+      </c>
+      <c r="U10" t="s">
+        <v>99</v>
+      </c>
+      <c r="V10" t="s" s="76">
+        <v>146</v>
+      </c>
+      <c r="W10" t="s" s="76">
+        <v>146</v>
+      </c>
+      <c r="X10" t="s" s="76">
+        <v>151</v>
+      </c>
+      <c r="Y10" t="s" s="76">
+        <v>147</v>
+      </c>
+      <c r="Z10" t="s" s="76">
+        <v>145</v>
+      </c>
+      <c r="AA10" t="s" s="76">
+        <v>145</v>
+      </c>
+      <c r="AB10" t="s" s="76">
+        <v>148</v>
+      </c>
+      <c r="AC10" t="s" s="76">
+        <v>146</v>
+      </c>
+      <c r="AD10" t="s" s="76">
+        <v>151</v>
+      </c>
+      <c r="AE10" t="s" s="76">
+        <v>146</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K11" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" t="s">
+        <v>98</v>
+      </c>
+      <c r="M11" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" t="s">
+        <v>98</v>
+      </c>
+      <c r="O11" t="s">
+        <v>98</v>
+      </c>
+      <c r="P11" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>98</v>
+      </c>
+      <c r="R11" t="s">
+        <v>98</v>
+      </c>
+      <c r="S11" t="s">
+        <v>99</v>
+      </c>
+      <c r="T11" t="s">
+        <v>98</v>
+      </c>
+      <c r="U11" t="s">
+        <v>98</v>
+      </c>
+      <c r="V11" t="s">
+        <v>98</v>
+      </c>
+      <c r="W11" t="s">
+        <v>98</v>
+      </c>
+      <c r="X11" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J12" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12" t="s">
+        <v>99</v>
+      </c>
+      <c r="L12" t="s">
+        <v>99</v>
+      </c>
+      <c r="M12" t="s">
+        <v>99</v>
+      </c>
+      <c r="N12" t="s">
+        <v>99</v>
+      </c>
+      <c r="O12" t="s">
+        <v>99</v>
+      </c>
+      <c r="P12" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>99</v>
+      </c>
+      <c r="R12" t="s">
+        <v>99</v>
+      </c>
+      <c r="S12" t="s">
+        <v>99</v>
+      </c>
+      <c r="T12" t="s">
+        <v>99</v>
+      </c>
+      <c r="U12" t="s">
+        <v>99</v>
+      </c>
+      <c r="V12" t="s">
+        <v>99</v>
+      </c>
+      <c r="W12" t="s">
+        <v>99</v>
+      </c>
+      <c r="X12" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" t="s">
+        <v>98</v>
+      </c>
+      <c r="M13" t="s">
+        <v>98</v>
+      </c>
+      <c r="N13" t="s">
+        <v>98</v>
+      </c>
+      <c r="O13" t="s">
+        <v>98</v>
+      </c>
+      <c r="P13" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>98</v>
+      </c>
+      <c r="R13" t="s">
+        <v>98</v>
+      </c>
+      <c r="S13" t="s">
+        <v>98</v>
+      </c>
+      <c r="T13" t="s">
+        <v>98</v>
+      </c>
+      <c r="U13" t="s">
+        <v>98</v>
+      </c>
+      <c r="V13" t="s">
+        <v>98</v>
+      </c>
+      <c r="W13" t="s">
+        <v>98</v>
+      </c>
+      <c r="X13" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y13" t="s" s="76">
+        <v>152</v>
+      </c>
+      <c r="Z13" t="s" s="76">
+        <v>152</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD13" t="s" s="76">
+        <v>153</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF13" t="s" s="76">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" t="s">
+        <v>98</v>
+      </c>
+      <c r="M14" t="s">
+        <v>98</v>
+      </c>
+      <c r="N14" t="s">
+        <v>98</v>
+      </c>
+      <c r="O14" t="s">
+        <v>98</v>
+      </c>
+      <c r="P14" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>98</v>
+      </c>
+      <c r="R14" t="s">
+        <v>99</v>
+      </c>
+      <c r="S14" t="s" s="76">
+        <v>155</v>
+      </c>
+      <c r="T14" t="s" s="76">
+        <v>156</v>
+      </c>
+      <c r="U14" t="s">
+        <v>98</v>
+      </c>
+      <c r="V14" t="s">
+        <v>98</v>
+      </c>
+      <c r="W14" t="s">
+        <v>98</v>
+      </c>
+      <c r="X14" t="s" s="76">
+        <v>155</v>
+      </c>
+      <c r="Y14" t="s" s="76">
+        <v>156</v>
+      </c>
+      <c r="Z14" t="s" s="76">
+        <v>157</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s" s="76">
+        <v>158</v>
+      </c>
+      <c r="D15" t="s" s="76">
+        <v>159</v>
+      </c>
+      <c r="E15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" t="s" s="76">
+        <v>160</v>
+      </c>
+      <c r="G15" t="s" s="76">
+        <v>159</v>
+      </c>
+      <c r="H15" t="s" s="76">
+        <v>161</v>
+      </c>
+      <c r="I15" t="s" s="76">
+        <v>160</v>
+      </c>
+      <c r="J15" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" t="s" s="76">
+        <v>159</v>
+      </c>
+      <c r="L15" t="s">
+        <v>99</v>
+      </c>
+      <c r="M15" t="s" s="76">
+        <v>158</v>
+      </c>
+      <c r="N15" t="s" s="76">
+        <v>161</v>
+      </c>
+      <c r="O15" t="s" s="76">
+        <v>162</v>
+      </c>
+      <c r="P15" t="s" s="76">
+        <v>163</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>99</v>
+      </c>
+      <c r="R15" t="s" s="76">
+        <v>159</v>
+      </c>
+      <c r="S15" t="s" s="76">
+        <v>164</v>
+      </c>
+      <c r="T15" t="s" s="76">
+        <v>161</v>
+      </c>
+      <c r="U15" t="s">
+        <v>98</v>
+      </c>
+      <c r="V15" t="s">
+        <v>98</v>
+      </c>
+      <c r="W15" t="s">
+        <v>98</v>
+      </c>
+      <c r="X15" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" t="s">
+        <v>98</v>
+      </c>
+      <c r="J16" t="s">
+        <v>98</v>
+      </c>
+      <c r="K16" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" t="s">
+        <v>98</v>
+      </c>
+      <c r="M16" t="s">
+        <v>98</v>
+      </c>
+      <c r="N16" t="s">
+        <v>98</v>
+      </c>
+      <c r="O16" t="s">
+        <v>98</v>
+      </c>
+      <c r="P16" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>98</v>
+      </c>
+      <c r="R16" t="s">
+        <v>98</v>
+      </c>
+      <c r="S16" t="s">
+        <v>98</v>
+      </c>
+      <c r="T16" t="s">
+        <v>98</v>
+      </c>
+      <c r="U16" t="s">
+        <v>98</v>
+      </c>
+      <c r="V16" t="s">
+        <v>98</v>
+      </c>
+      <c r="W16" t="s">
+        <v>98</v>
+      </c>
+      <c r="X16" t="s" s="76">
+        <v>165</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z16" t="s" s="76">
+        <v>166</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD16" t="s" s="76">
+        <v>165</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF16" t="s" s="76">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s" s="76">
+        <v>168</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" t="s" s="76">
+        <v>168</v>
+      </c>
+      <c r="F17" t="s" s="76">
+        <v>169</v>
+      </c>
+      <c r="G17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" t="s" s="76">
+        <v>170</v>
+      </c>
+      <c r="I17" t="s" s="76">
+        <v>170</v>
+      </c>
+      <c r="J17" t="s" s="76">
+        <v>168</v>
+      </c>
+      <c r="K17" t="s" s="76">
+        <v>169</v>
+      </c>
+      <c r="L17" t="s" s="76">
+        <v>168</v>
+      </c>
+      <c r="M17" t="s" s="76">
+        <v>168</v>
+      </c>
+      <c r="N17" t="s" s="76">
+        <v>171</v>
+      </c>
+      <c r="O17" t="s" s="76">
+        <v>170</v>
+      </c>
+      <c r="P17" t="s" s="76">
+        <v>168</v>
+      </c>
+      <c r="Q17" t="s" s="76">
+        <v>168</v>
+      </c>
+      <c r="R17" t="s" s="76">
+        <v>171</v>
+      </c>
+      <c r="S17" t="s" s="76">
+        <v>172</v>
+      </c>
+      <c r="T17" t="s">
+        <v>99</v>
+      </c>
+      <c r="U17" t="s" s="76">
+        <v>170</v>
+      </c>
+      <c r="V17" t="s" s="76">
+        <v>168</v>
+      </c>
+      <c r="W17" t="s" s="76">
+        <v>171</v>
+      </c>
+      <c r="X17" t="s" s="76">
+        <v>169</v>
+      </c>
+      <c r="Y17" t="s" s="76">
+        <v>173</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA17" t="s" s="76">
+        <v>170</v>
+      </c>
+      <c r="AB17" t="s" s="76">
+        <v>171</v>
+      </c>
+      <c r="AC17" t="s" s="76">
+        <v>172</v>
+      </c>
+      <c r="AD17" t="s" s="76">
+        <v>169</v>
+      </c>
+      <c r="AE17" t="s" s="76">
+        <v>168</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" t="s" s="76">
+        <v>174</v>
+      </c>
+      <c r="E18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" t="s" s="76">
+        <v>175</v>
+      </c>
+      <c r="G18" t="s" s="76">
+        <v>176</v>
+      </c>
+      <c r="H18" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" t="s">
+        <v>99</v>
+      </c>
+      <c r="J18" t="s" s="76">
+        <v>174</v>
+      </c>
+      <c r="K18" t="s" s="76">
+        <v>177</v>
+      </c>
+      <c r="L18" t="s">
+        <v>99</v>
+      </c>
+      <c r="M18" t="s" s="76">
+        <v>176</v>
+      </c>
+      <c r="N18" t="s" s="76">
+        <v>175</v>
+      </c>
+      <c r="O18" t="s" s="76">
+        <v>174</v>
+      </c>
+      <c r="P18" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>99</v>
+      </c>
+      <c r="R18" t="s" s="76">
+        <v>177</v>
+      </c>
+      <c r="S18" t="s">
+        <v>98</v>
+      </c>
+      <c r="T18" t="s" s="76">
+        <v>176</v>
+      </c>
+      <c r="U18" t="s" s="76">
+        <v>176</v>
+      </c>
+      <c r="V18" t="s">
+        <v>99</v>
+      </c>
+      <c r="W18" t="s" s="76">
+        <v>175</v>
+      </c>
+      <c r="X18" t="s" s="76">
+        <v>177</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB18" t="s" s="76">
+        <v>175</v>
+      </c>
+      <c r="AC18" t="s" s="76">
+        <v>177</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE18" t="s" s="76">
+        <v>178</v>
+      </c>
+      <c r="AF18" t="s" s="76">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="O1:T1"/>
+    <mergeCell ref="U1:Z1"/>
+    <mergeCell ref="AA1:AF1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>